<commit_message>
Remove outdated Rplots.pdf and test_output.html files. Update author and date metadata in analysis documents. Enhance the introduction section with project purpose, significance, and scientific foundation. Revise statistical analysis results and improve formatting in CSV files for clarity.
</commit_message>
<xml_diff>
--- a/metadata/PS2720_xtra_samples_HMM Submission Sheet.xlsx
+++ b/metadata/PS2720_xtra_samples_HMM Submission Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\DFI Metabolomics Lab\03_Science\05_Collaborations\71_Patrick Seed\PS2720\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pseed\Documents\GitHub\abbott-carbohydrate-obesity-project2\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69EE3875-47D6-428A-8A96-28DF5126E65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DE382E-6C76-485A-8B3D-4DE970177462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="99">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>PFBBr(SCFA) Panel              (Yes/No)</t>
-  </si>
-  <si>
-    <t>case</t>
   </si>
   <si>
     <t>control</t>
@@ -863,15 +860,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1364,7 +1361,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1408,7 +1405,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1432,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:OG449"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:A293"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
@@ -1469,25 +1466,25 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="66"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="68"/>
       <c r="U2" s="42" t="s">
         <v>14</v>
       </c>
@@ -5851,8 +5848,8 @@
       <c r="OG13" s="24"/>
     </row>
     <row r="14" spans="1:397" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="67" t="s">
-        <v>60</v>
+      <c r="A14" s="65" t="s">
+        <v>59</v>
       </c>
       <c r="B14" s="38" t="s">
         <v>57</v>
@@ -5888,7 +5885,7 @@
         <v>34</v>
       </c>
       <c r="M14" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N14" s="38" t="s">
         <v>35</v>
@@ -6290,8 +6287,8 @@
       <c r="OG14" s="24"/>
     </row>
     <row r="15" spans="1:397" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="68" t="s">
-        <v>61</v>
+      <c r="A15" s="66" t="s">
+        <v>60</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>57</v>
@@ -6327,7 +6324,7 @@
         <v>34</v>
       </c>
       <c r="M15" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N15" s="38" t="s">
         <v>35</v>
@@ -6375,8 +6372,8 @@
       <c r="AQ15" s="50"/>
     </row>
     <row r="16" spans="1:397" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="68" t="s">
-        <v>62</v>
+      <c r="A16" s="66" t="s">
+        <v>61</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>57</v>
@@ -6412,7 +6409,7 @@
         <v>34</v>
       </c>
       <c r="M16" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N16" s="38" t="s">
         <v>35</v>
@@ -6460,8 +6457,8 @@
       <c r="AQ16" s="50"/>
     </row>
     <row r="17" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="68" t="s">
-        <v>63</v>
+      <c r="A17" s="66" t="s">
+        <v>62</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>57</v>
@@ -6497,7 +6494,7 @@
         <v>34</v>
       </c>
       <c r="M17" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N17" s="38" t="s">
         <v>35</v>
@@ -6545,8 +6542,8 @@
       <c r="AQ17" s="50"/>
     </row>
     <row r="18" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="68" t="s">
-        <v>64</v>
+      <c r="A18" s="66" t="s">
+        <v>63</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>57</v>
@@ -6582,7 +6579,7 @@
         <v>34</v>
       </c>
       <c r="M18" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N18" s="38" t="s">
         <v>35</v>
@@ -6630,8 +6627,8 @@
       <c r="AQ18" s="50"/>
     </row>
     <row r="19" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="68" t="s">
-        <v>65</v>
+      <c r="A19" s="66" t="s">
+        <v>64</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>57</v>
@@ -6667,7 +6664,7 @@
         <v>34</v>
       </c>
       <c r="M19" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N19" s="38" t="s">
         <v>35</v>
@@ -6715,8 +6712,8 @@
       <c r="AQ19" s="50"/>
     </row>
     <row r="20" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="68" t="s">
-        <v>66</v>
+      <c r="A20" s="66" t="s">
+        <v>65</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>57</v>
@@ -6752,7 +6749,7 @@
         <v>34</v>
       </c>
       <c r="M20" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N20" s="38" t="s">
         <v>35</v>
@@ -6800,8 +6797,8 @@
       <c r="AQ20" s="50"/>
     </row>
     <row r="21" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="68" t="s">
-        <v>67</v>
+      <c r="A21" s="66" t="s">
+        <v>66</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>57</v>
@@ -6837,7 +6834,7 @@
         <v>34</v>
       </c>
       <c r="M21" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N21" s="38" t="s">
         <v>35</v>
@@ -6885,8 +6882,8 @@
       <c r="AQ21" s="50"/>
     </row>
     <row r="22" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="68" t="s">
-        <v>68</v>
+      <c r="A22" s="66" t="s">
+        <v>67</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>57</v>
@@ -6922,7 +6919,7 @@
         <v>34</v>
       </c>
       <c r="M22" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N22" s="38" t="s">
         <v>35</v>
@@ -6970,8 +6967,8 @@
       <c r="AQ22" s="50"/>
     </row>
     <row r="23" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="68" t="s">
-        <v>69</v>
+      <c r="A23" s="66" t="s">
+        <v>68</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>57</v>
@@ -7007,7 +7004,7 @@
         <v>34</v>
       </c>
       <c r="M23" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N23" s="38" t="s">
         <v>35</v>
@@ -7055,8 +7052,8 @@
       <c r="AQ23" s="50"/>
     </row>
     <row r="24" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="68" t="s">
-        <v>70</v>
+      <c r="A24" s="66" t="s">
+        <v>69</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>57</v>
@@ -7092,7 +7089,7 @@
         <v>34</v>
       </c>
       <c r="M24" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N24" s="38" t="s">
         <v>35</v>
@@ -7140,8 +7137,8 @@
       <c r="AQ24" s="50"/>
     </row>
     <row r="25" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="68" t="s">
-        <v>71</v>
+      <c r="A25" s="66" t="s">
+        <v>70</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>57</v>
@@ -7177,7 +7174,7 @@
         <v>34</v>
       </c>
       <c r="M25" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N25" s="38" t="s">
         <v>35</v>
@@ -7225,8 +7222,8 @@
       <c r="AQ25" s="50"/>
     </row>
     <row r="26" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="68" t="s">
-        <v>72</v>
+      <c r="A26" s="66" t="s">
+        <v>71</v>
       </c>
       <c r="B26" s="38" t="s">
         <v>57</v>
@@ -7262,7 +7259,7 @@
         <v>34</v>
       </c>
       <c r="M26" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N26" s="38" t="s">
         <v>35</v>
@@ -7310,8 +7307,8 @@
       <c r="AQ26" s="50"/>
     </row>
     <row r="27" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="68" t="s">
-        <v>73</v>
+      <c r="A27" s="66" t="s">
+        <v>72</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>57</v>
@@ -7347,7 +7344,7 @@
         <v>34</v>
       </c>
       <c r="M27" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N27" s="38" t="s">
         <v>35</v>
@@ -7395,8 +7392,8 @@
       <c r="AQ27" s="50"/>
     </row>
     <row r="28" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="68" t="s">
-        <v>74</v>
+      <c r="A28" s="66" t="s">
+        <v>73</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>57</v>
@@ -7432,7 +7429,7 @@
         <v>34</v>
       </c>
       <c r="M28" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N28" s="38" t="s">
         <v>35</v>
@@ -7480,8 +7477,8 @@
       <c r="AQ28" s="50"/>
     </row>
     <row r="29" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="68" t="s">
-        <v>75</v>
+      <c r="A29" s="66" t="s">
+        <v>74</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>57</v>
@@ -7517,7 +7514,7 @@
         <v>34</v>
       </c>
       <c r="M29" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N29" s="38" t="s">
         <v>35</v>
@@ -7565,8 +7562,8 @@
       <c r="AQ29" s="50"/>
     </row>
     <row r="30" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="68" t="s">
-        <v>76</v>
+      <c r="A30" s="66" t="s">
+        <v>75</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>57</v>
@@ -7602,7 +7599,7 @@
         <v>34</v>
       </c>
       <c r="M30" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N30" s="38" t="s">
         <v>35</v>
@@ -7650,8 +7647,8 @@
       <c r="AQ30" s="50"/>
     </row>
     <row r="31" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="68" t="s">
-        <v>77</v>
+      <c r="A31" s="66" t="s">
+        <v>76</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>57</v>
@@ -7687,7 +7684,7 @@
         <v>34</v>
       </c>
       <c r="M31" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N31" s="38" t="s">
         <v>35</v>
@@ -7735,8 +7732,8 @@
       <c r="AQ31" s="50"/>
     </row>
     <row r="32" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="68" t="s">
-        <v>78</v>
+      <c r="A32" s="66" t="s">
+        <v>77</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>57</v>
@@ -7772,7 +7769,7 @@
         <v>34</v>
       </c>
       <c r="M32" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N32" s="38" t="s">
         <v>35</v>
@@ -7820,8 +7817,8 @@
       <c r="AQ32" s="50"/>
     </row>
     <row r="33" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="68" t="s">
-        <v>79</v>
+      <c r="A33" s="66" t="s">
+        <v>78</v>
       </c>
       <c r="B33" s="38" t="s">
         <v>57</v>
@@ -7857,7 +7854,7 @@
         <v>34</v>
       </c>
       <c r="M33" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N33" s="38" t="s">
         <v>35</v>
@@ -7905,11 +7902,11 @@
       <c r="AQ33" s="50"/>
     </row>
     <row r="34" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="68" t="s">
-        <v>80</v>
+      <c r="A34" s="66" t="s">
+        <v>79</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="38" t="s">
         <v>50</v>
@@ -7942,7 +7939,7 @@
         <v>34</v>
       </c>
       <c r="M34" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N34" s="38" t="s">
         <v>35</v>
@@ -7990,11 +7987,11 @@
       <c r="AQ34" s="50"/>
     </row>
     <row r="35" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="68" t="s">
-        <v>81</v>
+      <c r="A35" s="66" t="s">
+        <v>80</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="38" t="s">
         <v>50</v>
@@ -8027,7 +8024,7 @@
         <v>34</v>
       </c>
       <c r="M35" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N35" s="38" t="s">
         <v>35</v>
@@ -8075,11 +8072,11 @@
       <c r="AQ35" s="50"/>
     </row>
     <row r="36" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="68" t="s">
-        <v>82</v>
+      <c r="A36" s="66" t="s">
+        <v>81</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>50</v>
@@ -8112,7 +8109,7 @@
         <v>34</v>
       </c>
       <c r="M36" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N36" s="38" t="s">
         <v>35</v>
@@ -8160,11 +8157,11 @@
       <c r="AQ36" s="50"/>
     </row>
     <row r="37" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="68" t="s">
-        <v>83</v>
+      <c r="A37" s="66" t="s">
+        <v>82</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>50</v>
@@ -8197,7 +8194,7 @@
         <v>34</v>
       </c>
       <c r="M37" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N37" s="38" t="s">
         <v>35</v>
@@ -8245,11 +8242,11 @@
       <c r="AQ37" s="50"/>
     </row>
     <row r="38" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="68" t="s">
-        <v>84</v>
+      <c r="A38" s="66" t="s">
+        <v>83</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="38" t="s">
         <v>50</v>
@@ -8282,7 +8279,7 @@
         <v>34</v>
       </c>
       <c r="M38" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N38" s="38" t="s">
         <v>35</v>
@@ -8330,11 +8327,11 @@
       <c r="AQ38" s="50"/>
     </row>
     <row r="39" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A39" s="68" t="s">
-        <v>85</v>
+      <c r="A39" s="66" t="s">
+        <v>84</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="38" t="s">
         <v>50</v>
@@ -8367,7 +8364,7 @@
         <v>34</v>
       </c>
       <c r="M39" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N39" s="38" t="s">
         <v>35</v>
@@ -8415,11 +8412,11 @@
       <c r="AQ39" s="50"/>
     </row>
     <row r="40" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="68" t="s">
-        <v>86</v>
+      <c r="A40" s="66" t="s">
+        <v>85</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="38" t="s">
         <v>50</v>
@@ -8452,7 +8449,7 @@
         <v>34</v>
       </c>
       <c r="M40" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N40" s="38" t="s">
         <v>35</v>
@@ -8500,11 +8497,11 @@
       <c r="AQ40" s="50"/>
     </row>
     <row r="41" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="68" t="s">
-        <v>87</v>
+      <c r="A41" s="66" t="s">
+        <v>86</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="38" t="s">
         <v>50</v>
@@ -8537,7 +8534,7 @@
         <v>34</v>
       </c>
       <c r="M41" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N41" s="38" t="s">
         <v>35</v>
@@ -8585,11 +8582,11 @@
       <c r="AQ41" s="50"/>
     </row>
     <row r="42" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="68" t="s">
-        <v>88</v>
+      <c r="A42" s="66" t="s">
+        <v>87</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>50</v>
@@ -8622,7 +8619,7 @@
         <v>34</v>
       </c>
       <c r="M42" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N42" s="38" t="s">
         <v>35</v>
@@ -8670,11 +8667,11 @@
       <c r="AQ42" s="50"/>
     </row>
     <row r="43" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="68" t="s">
-        <v>89</v>
+      <c r="A43" s="66" t="s">
+        <v>88</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>50</v>
@@ -8707,7 +8704,7 @@
         <v>34</v>
       </c>
       <c r="M43" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N43" s="38" t="s">
         <v>35</v>
@@ -8755,11 +8752,11 @@
       <c r="AQ43" s="50"/>
     </row>
     <row r="44" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="68" t="s">
-        <v>90</v>
+      <c r="A44" s="66" t="s">
+        <v>89</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" s="38" t="s">
         <v>50</v>
@@ -8792,7 +8789,7 @@
         <v>34</v>
       </c>
       <c r="M44" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N44" s="38" t="s">
         <v>35</v>
@@ -8840,11 +8837,11 @@
       <c r="AQ44" s="50"/>
     </row>
     <row r="45" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A45" s="68" t="s">
-        <v>91</v>
+      <c r="A45" s="66" t="s">
+        <v>90</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="38" t="s">
         <v>50</v>
@@ -8877,7 +8874,7 @@
         <v>34</v>
       </c>
       <c r="M45" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N45" s="38" t="s">
         <v>35</v>
@@ -8925,11 +8922,11 @@
       <c r="AQ45" s="50"/>
     </row>
     <row r="46" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="68" t="s">
-        <v>92</v>
+      <c r="A46" s="66" t="s">
+        <v>91</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="38" t="s">
         <v>50</v>
@@ -8962,7 +8959,7 @@
         <v>34</v>
       </c>
       <c r="M46" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N46" s="38" t="s">
         <v>35</v>
@@ -9010,11 +9007,11 @@
       <c r="AQ46" s="50"/>
     </row>
     <row r="47" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A47" s="68" t="s">
-        <v>93</v>
+      <c r="A47" s="66" t="s">
+        <v>92</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>50</v>
@@ -9047,7 +9044,7 @@
         <v>34</v>
       </c>
       <c r="M47" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N47" s="38" t="s">
         <v>35</v>
@@ -9095,11 +9092,11 @@
       <c r="AQ47" s="50"/>
     </row>
     <row r="48" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A48" s="68" t="s">
-        <v>94</v>
+      <c r="A48" s="66" t="s">
+        <v>93</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="38" t="s">
         <v>50</v>
@@ -9132,7 +9129,7 @@
         <v>34</v>
       </c>
       <c r="M48" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N48" s="38" t="s">
         <v>35</v>
@@ -9180,11 +9177,11 @@
       <c r="AQ48" s="50"/>
     </row>
     <row r="49" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="68" t="s">
-        <v>95</v>
+      <c r="A49" s="66" t="s">
+        <v>94</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="38" t="s">
         <v>50</v>
@@ -9217,7 +9214,7 @@
         <v>34</v>
       </c>
       <c r="M49" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N49" s="38" t="s">
         <v>35</v>
@@ -9265,11 +9262,11 @@
       <c r="AQ49" s="50"/>
     </row>
     <row r="50" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A50" s="68" t="s">
-        <v>96</v>
+      <c r="A50" s="66" t="s">
+        <v>95</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" s="38" t="s">
         <v>50</v>
@@ -9302,7 +9299,7 @@
         <v>34</v>
       </c>
       <c r="M50" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N50" s="38" t="s">
         <v>35</v>
@@ -9350,11 +9347,11 @@
       <c r="AQ50" s="50"/>
     </row>
     <row r="51" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A51" s="68" t="s">
-        <v>97</v>
+      <c r="A51" s="66" t="s">
+        <v>96</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51" s="38" t="s">
         <v>50</v>
@@ -9387,7 +9384,7 @@
         <v>34</v>
       </c>
       <c r="M51" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N51" s="38" t="s">
         <v>35</v>
@@ -9435,11 +9432,11 @@
       <c r="AQ51" s="50"/>
     </row>
     <row r="52" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="68" t="s">
-        <v>98</v>
+      <c r="A52" s="66" t="s">
+        <v>97</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" s="38" t="s">
         <v>50</v>
@@ -9472,7 +9469,7 @@
         <v>34</v>
       </c>
       <c r="M52" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N52" s="38" t="s">
         <v>35</v>
@@ -9520,11 +9517,11 @@
       <c r="AQ52" s="50"/>
     </row>
     <row r="53" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="68" t="s">
-        <v>99</v>
+      <c r="A53" s="66" t="s">
+        <v>98</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="38" t="s">
         <v>50</v>
@@ -9557,7 +9554,7 @@
         <v>34</v>
       </c>
       <c r="M53" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N53" s="38" t="s">
         <v>35</v>

</xml_diff>